<commit_message>
code for added new changfes
</commit_message>
<xml_diff>
--- a/templates/Time_Table_Template.xlsx
+++ b/templates/Time_Table_Template.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Time Table Template" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -33,6 +36,9 @@
   </si>
   <si>
     <t>Topic</t>
+  </si>
+  <si>
+    <t>Trainer</t>
   </si>
 </sst>
 </file>
@@ -81,8 +87,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -357,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -375,6 +409,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>